<commit_message>
added alternative for calculating PE
</commit_message>
<xml_diff>
--- a/stockdata.xlsx
+++ b/stockdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,143 +458,161 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>IVV</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>177.5700073242188</v>
+        <v>432.7099914550781</v>
       </c>
       <c r="C2" t="n">
-        <v>39.509033203125</v>
+        <v>66.1177978515625</v>
       </c>
       <c r="D2" t="n">
-        <v>29.79</v>
+        <v>21.71</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TSLA</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>218.5099945068359</v>
+        <v>395.7799987792969</v>
       </c>
       <c r="C3" t="n">
-        <v>3.199996948242188</v>
+        <v>60.5667724609375</v>
       </c>
       <c r="D3" t="n">
-        <v>70.48999999999999</v>
+        <v>21.56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>348.3200073242188</v>
+        <v>213.0099945068359</v>
       </c>
       <c r="C4" t="n">
-        <v>136.1200408935547</v>
+        <v>29.48443603515625</v>
       </c>
       <c r="D4" t="n">
-        <v>33.75</v>
+        <v>20.03</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GOOGL</t>
+          <t>QQQ</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>127.4899978637695</v>
+        <v>363.4400024414062</v>
       </c>
       <c r="C5" t="n">
-        <v>44.05999755859375</v>
+        <v>104.7037963867188</v>
       </c>
       <c r="D5" t="n">
-        <v>24.42</v>
+        <v>29.64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>VTV</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>435.0599975585938</v>
+        <v>137.3999938964844</v>
       </c>
       <c r="C6" t="n">
-        <v>300.9320373535156</v>
+        <v>5.09356689453125</v>
       </c>
       <c r="D6" t="n">
-        <v>105.09</v>
+        <v>15.36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>META</t>
+          <t>VUG</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>310.8699951171875</v>
+        <v>276.8900146484375</v>
       </c>
       <c r="C7" t="n">
-        <v>221.9599914550781</v>
+        <v>69.81861877441406</v>
       </c>
       <c r="D7" t="n">
-        <v>27.44</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NFLX</t>
+          <t>IWF</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>424.7099914550781</v>
+        <v>271.0299987792969</v>
       </c>
       <c r="C8" t="n">
-        <v>155.6499938964844</v>
+        <v>62.83857727050781</v>
       </c>
       <c r="D8" t="n">
-        <v>42.39</v>
+        <v>29.92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>VIG</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37.70000076293945</v>
+        <v>156.5899963378906</v>
       </c>
       <c r="C9" t="n">
-        <v>11.20454597473145</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+        <v>15.28024291992188</v>
+      </c>
+      <c r="D9" t="n">
+        <v>22.04</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AMZN</t>
+          <t>IJH</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>138.0700073242188</v>
+        <v>242.5599975585938</v>
       </c>
       <c r="C10" t="n">
-        <v>48.77000427246094</v>
+        <v>10.45112609863281</v>
       </c>
       <c r="D10" t="n">
-        <v>72.31</v>
+        <v>13.36</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>IJR</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>91.66000366210938</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-1.283927917480469</v>
+      </c>
+      <c r="D11" t="n">
+        <v>11.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ETF Analysis + percent change code edit
</commit_message>
<xml_diff>
--- a/stockdata.xlsx
+++ b/stockdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,159 +458,1493 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>MSOS</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>175.7301940917969</v>
+        <v>5.880000114440918</v>
       </c>
       <c r="C2" t="n">
-        <v>37.66921997070312</v>
-      </c>
-      <c r="D2" t="n">
-        <v>29.44</v>
-      </c>
+        <v>-5.119999885559082</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TSLA</t>
+          <t>ARKK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>222.5009002685547</v>
+        <v>40.43999862670898</v>
       </c>
       <c r="C3" t="n">
-        <v>7.190902709960938</v>
-      </c>
-      <c r="D3" t="n">
-        <v>71.79000000000001</v>
-      </c>
+        <v>5.511295318603516</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>AVUV</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>350.439208984375</v>
+        <v>78.62999725341797</v>
       </c>
       <c r="C4" t="n">
-        <v>138.2392272949219</v>
+        <v>4.059097290039062</v>
       </c>
       <c r="D4" t="n">
-        <v>33.99</v>
+        <v>6.79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GOOGL</t>
+          <t>LCTU</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>128.6499938964844</v>
+        <v>47.61000061035156</v>
       </c>
       <c r="C5" t="n">
-        <v>45.23999786376953</v>
+        <v>6.427463531494141</v>
       </c>
       <c r="D5" t="n">
-        <v>24.7</v>
+        <v>21.13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>XLC</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>442.885009765625</v>
+        <v>67.55999755859375</v>
       </c>
       <c r="C6" t="n">
-        <v>308.7570495605469</v>
+        <v>22.26338577270508</v>
       </c>
       <c r="D6" t="n">
-        <v>107.24</v>
+        <v>25.51</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>META</t>
+          <t>XLY</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>312.2200012207031</v>
+        <v>160.2200012207031</v>
       </c>
       <c r="C7" t="n">
-        <v>223.3049926757812</v>
+        <v>24.02964782714844</v>
       </c>
       <c r="D7" t="n">
-        <v>27.58</v>
+        <v>25.02</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NFLX</t>
+          <t>XLP</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>430.4800109863281</v>
+        <v>68.75</v>
       </c>
       <c r="C8" t="n">
-        <v>161.4200134277344</v>
+        <v>-1.272453308105469</v>
       </c>
       <c r="D8" t="n">
-        <v>42.96</v>
+        <v>23.44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>XLE</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37.75500106811523</v>
+        <v>86.68000030517578</v>
       </c>
       <c r="C9" t="n">
-        <v>11.25954818725586</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+        <v>-1.441215515136719</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8.02</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AMZN</t>
+          <t>XLF</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>137.7920074462891</v>
+        <v>33.77999877929688</v>
       </c>
       <c r="C10" t="n">
-        <v>48.49200439453125</v>
+        <v>0.5460777282714844</v>
       </c>
       <c r="D10" t="n">
-        <v>72.14</v>
+        <v>15.33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ORCL</t>
+          <t>GRID</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>108.375</v>
+        <v>89.88999938964844</v>
       </c>
       <c r="C11" t="n">
-        <v>34.4677734375</v>
+        <v>6.5155029296875</v>
       </c>
       <c r="D11" t="n">
-        <v>32.16</v>
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FAN</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>14.32999992370605</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-1.362451553344727</v>
+      </c>
+      <c r="D12" t="n">
+        <v>13.19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PAVE</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>30.13999938964844</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4.385295867919922</v>
+      </c>
+      <c r="D13" t="n">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>XLV</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>127.4100036621094</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-1.29730224609375</v>
+      </c>
+      <c r="D14" t="n">
+        <v>21.59</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>XLI</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>101.5999984741211</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8.12432861328125</v>
+      </c>
+      <c r="D15" t="n">
+        <v>21.82</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>QQQ</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>367.7099914550781</v>
+      </c>
+      <c r="C16" t="n">
+        <v>104.81201171875</v>
+      </c>
+      <c r="D16" t="n">
+        <v>29.98</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>RSP</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>141.5899963378906</v>
+      </c>
+      <c r="C17" t="n">
+        <v>6.10919189453125</v>
+      </c>
+      <c r="D17" t="n">
+        <v>18.02</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TAN</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>44.70000076293945</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-27.65999984741211</v>
+      </c>
+      <c r="D18" t="n">
+        <v>10.2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PHO</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>53.2400016784668</v>
+      </c>
+      <c r="C19" t="n">
+        <v>4.778335571289062</v>
+      </c>
+      <c r="D19" t="n">
+        <v>28.74</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PBW</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>27</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-16.28013610839844</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SHY</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>81.20999908447266</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2.771461486816406</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3691.36</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>IGSB</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>49.95999908447266</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2.388416290283203</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>TLT</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>87.62999725341797</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-3.570449829101562</v>
+      </c>
+      <c r="D23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>IEF</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>91.62999725341797</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.7673416137695312</v>
+      </c>
+      <c r="D24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>IBB</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>119.7900009155273</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-8.219352722167969</v>
+      </c>
+      <c r="D25" t="n">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>DGRO</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>49.84000015258789</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2.549980163574219</v>
+      </c>
+      <c r="D26" t="n">
+        <v>16.98</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>IEFA</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>65</v>
+      </c>
+      <c r="C27" t="n">
+        <v>9.333873748779297</v>
+      </c>
+      <c r="D27" t="n">
+        <v>13.02</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>IEMG</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>48.13999938964844</v>
+      </c>
+      <c r="C28" t="n">
+        <v>4.465198516845703</v>
+      </c>
+      <c r="D28" t="n">
+        <v>10.94</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>IVV</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>436.5899963378906</v>
+      </c>
+      <c r="C29" t="n">
+        <v>64.81231689453125</v>
+      </c>
+      <c r="D29" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>IJH</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>247.3000030517578</v>
+      </c>
+      <c r="C30" t="n">
+        <v>11.22453308105469</v>
+      </c>
+      <c r="D30" t="n">
+        <v>13.62</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>IJR</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>94.22000122070312</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-0.1801834106445312</v>
+      </c>
+      <c r="D31" t="n">
+        <v>11.65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>IUSB</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>43.75</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1.571475982666016</v>
+      </c>
+      <c r="D32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>AGG</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>94.18000030517578</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2.704017639160156</v>
+      </c>
+      <c r="D33" t="n">
+        <v>120.13</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ESGU</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>95.36000061035156</v>
+      </c>
+      <c r="C34" t="n">
+        <v>13.27500152587891</v>
+      </c>
+      <c r="D34" t="n">
+        <v>21.93</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ICLN</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>13.67000007629395</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-5.329006195068359</v>
+      </c>
+      <c r="D35" t="n">
+        <v>14.72</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>HYG</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>74.41000366210938</v>
+      </c>
+      <c r="C36" t="n">
+        <v>5.715110778808594</v>
+      </c>
+      <c r="D36" t="n">
+        <v>9.279999999999999</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>LQD</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>101.9100036621094</v>
+      </c>
+      <c r="C37" t="n">
+        <v>4.792160034179688</v>
+      </c>
+      <c r="D37" t="n">
+        <v>30.82</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ESGE</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>30.89999961853027</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2.874490737915039</v>
+      </c>
+      <c r="D38" t="n">
+        <v>11.31</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>EMB</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>83.51999664306641</v>
+      </c>
+      <c r="C39" t="n">
+        <v>6.973091125488281</v>
+      </c>
+      <c r="D39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>MBB</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>88.91000366210938</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1.832321166992188</v>
+      </c>
+      <c r="D40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>EWA</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>21.80999946594238</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1.259576797485352</v>
+      </c>
+      <c r="D41" t="n">
+        <v>12.94</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>EWZ</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>31.89999961853027</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.141880035400391</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>MCHI</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>43.25</v>
+      </c>
+      <c r="C43" t="n">
+        <v>3.533542633056641</v>
+      </c>
+      <c r="D43" t="n">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>EFA</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>69.66000366210938</v>
+      </c>
+      <c r="C44" t="n">
+        <v>10.24179077148438</v>
+      </c>
+      <c r="D44" t="n">
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>INDA</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>44.15000152587891</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1.171516418457031</v>
+      </c>
+      <c r="D45" t="n">
+        <v>24.42</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>DSI</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>82.5</v>
+      </c>
+      <c r="C46" t="n">
+        <v>13.54653930664062</v>
+      </c>
+      <c r="D46" t="n">
+        <v>24.52</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>EWW</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>59.52999877929688</v>
+      </c>
+      <c r="C47" t="n">
+        <v>8.150421142578125</v>
+      </c>
+      <c r="D47" t="n">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>EWT</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>45.7400016784668</v>
+      </c>
+      <c r="C48" t="n">
+        <v>9.269321441650391</v>
+      </c>
+      <c r="D48" t="n">
+        <v>12.87</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>USMV</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>73.72000122070312</v>
+      </c>
+      <c r="C49" t="n">
+        <v>5.209556579589844</v>
+      </c>
+      <c r="D49" t="n">
+        <v>23.19</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>MTUM</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>143.75</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.630126953125</v>
+      </c>
+      <c r="D50" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>QUAL</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>134.9900054931641</v>
+      </c>
+      <c r="C51" t="n">
+        <v>26.37348937988281</v>
+      </c>
+      <c r="D51" t="n">
+        <v>19.91</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>MUB</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>102.7600021362305</v>
+      </c>
+      <c r="C52" t="n">
+        <v>3.523262023925781</v>
+      </c>
+      <c r="D52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>IWF</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>273.6400146484375</v>
+      </c>
+      <c r="C53" t="n">
+        <v>63.31600952148438</v>
+      </c>
+      <c r="D53" t="n">
+        <v>30.21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>IWD</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>151.8300018310547</v>
+      </c>
+      <c r="C54" t="n">
+        <v>6.307769775390625</v>
+      </c>
+      <c r="D54" t="n">
+        <v>15.79</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>IWM</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>174.4900054931641</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-1.400604248046875</v>
+      </c>
+      <c r="D55" t="n">
+        <v>11.13</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>SHV</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>110.1500015258789</v>
+      </c>
+      <c r="C56" t="n">
+        <v>5.037483215332031</v>
+      </c>
+      <c r="D56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>TIP</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>104.2399978637695</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1.964340209960938</v>
+      </c>
+      <c r="D57" t="n">
+        <v>11.71</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ESGD</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>69.65000152587891</v>
+      </c>
+      <c r="C58" t="n">
+        <v>10.247314453125</v>
+      </c>
+      <c r="D58" t="n">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ITA</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>113.4199981689453</v>
+      </c>
+      <c r="C59" t="n">
+        <v>7.199058532714844</v>
+      </c>
+      <c r="D59" t="n">
+        <v>26.11</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GOVT</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>22.07999992370605</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.4086074829101562</v>
+      </c>
+      <c r="D60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>IYW</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>108.629997253418</v>
+      </c>
+      <c r="C61" t="n">
+        <v>37.27071380615234</v>
+      </c>
+      <c r="D61" t="n">
+        <v>32.91</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>BBCA</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>58.81999969482422</v>
+      </c>
+      <c r="C62" t="n">
+        <v>2.429946899414062</v>
+      </c>
+      <c r="D62" t="n">
+        <v>13.23</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>JEPI</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>53.59000015258789</v>
+      </c>
+      <c r="C63" t="n">
+        <v>3.172592163085938</v>
+      </c>
+      <c r="D63" t="n">
+        <v>23.37</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>JPST</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>50.06000137329102</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1.685844421386719</v>
+      </c>
+      <c r="D64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>COWZ</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>49.56999969482422</v>
+      </c>
+      <c r="C65" t="n">
+        <v>3.722404479980469</v>
+      </c>
+      <c r="D65" t="n">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>NOBL</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>88.01000213623047</v>
+      </c>
+      <c r="C66" t="n">
+        <v>2.395439147949219</v>
+      </c>
+      <c r="D66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>IPO</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>31.80999946594238</v>
+      </c>
+      <c r="C67" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="D67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>SCHD</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>70.25</v>
+      </c>
+      <c r="C68" t="n">
+        <v>-0.6469039916992188</v>
+      </c>
+      <c r="D68" t="n">
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>BIL</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>91.48000335693359</v>
+      </c>
+      <c r="C69" t="n">
+        <v>4.101837158203125</v>
+      </c>
+      <c r="D69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>434.6900024414062</v>
+      </c>
+      <c r="C70" t="n">
+        <v>64.17276000976562</v>
+      </c>
+      <c r="D70" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>XLK</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>171.7599945068359</v>
+      </c>
+      <c r="C71" t="n">
+        <v>51.88980102539062</v>
+      </c>
+      <c r="D71" t="n">
+        <v>32.54</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>XLU</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>61.86000061035156</v>
+      </c>
+      <c r="C72" t="n">
+        <v>-3.144767761230469</v>
+      </c>
+      <c r="D72" t="n">
+        <v>21.76</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>MOAT</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>75.30999755859375</v>
+      </c>
+      <c r="C73" t="n">
+        <v>14.03970336914062</v>
+      </c>
+      <c r="D73" t="n">
+        <v>23.97</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>SMH</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>149.5099945068359</v>
+      </c>
+      <c r="C74" t="n">
+        <v>54.88582611083984</v>
+      </c>
+      <c r="D74" t="n">
+        <v>12.93</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>VIG</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>157.7400054931641</v>
+      </c>
+      <c r="C75" t="n">
+        <v>14.30448913574219</v>
+      </c>
+      <c r="D75" t="n">
+        <v>22.21</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>ESGV</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>76.45999908447266</v>
+      </c>
+      <c r="C76" t="n">
+        <v>12.44647979736328</v>
+      </c>
+      <c r="D76" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>VEU</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>52.43999862670898</v>
+      </c>
+      <c r="C77" t="n">
+        <v>6.538074493408203</v>
+      </c>
+      <c r="D77" t="n">
+        <v>11.97</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>VEA</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>44.18999862670898</v>
+      </c>
+      <c r="C78" t="n">
+        <v>5.960304260253906</v>
+      </c>
+      <c r="D78" t="n">
+        <v>12.17</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>VWO</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>39.5099983215332</v>
+      </c>
+      <c r="C79" t="n">
+        <v>3.106521606445312</v>
+      </c>
+      <c r="D79" t="n">
+        <v>10.76</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>VGK</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>58.2400016784668</v>
+      </c>
+      <c r="C80" t="n">
+        <v>8.653209686279297</v>
+      </c>
+      <c r="D80" t="n">
+        <v>12.53</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>VUG</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>279.8900146484375</v>
+      </c>
+      <c r="C81" t="n">
+        <v>70.1068115234375</v>
+      </c>
+      <c r="D81" t="n">
+        <v>33.69</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>VHT</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>231.4600067138672</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-4.19696044921875</v>
+      </c>
+      <c r="D82" t="n">
+        <v>20.99</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>VYM</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>103.8199996948242</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.5161666870117188</v>
+      </c>
+      <c r="D83" t="n">
+        <v>14.22</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>VGT</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>427.8800048828125</v>
+      </c>
+      <c r="C84" t="n">
+        <v>119.9217529296875</v>
+      </c>
+      <c r="D84" t="n">
+        <v>31.74</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>VCIT</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>76.05000305175781</v>
+      </c>
+      <c r="C85" t="n">
+        <v>3.864532470703125</v>
+      </c>
+      <c r="D85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>VO</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>207.8000030517578</v>
+      </c>
+      <c r="C86" t="n">
+        <v>10.20899963378906</v>
+      </c>
+      <c r="D86" t="n">
+        <v>16.87</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>VNQ</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>77.58999633789062</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-0.4830703735351562</v>
+      </c>
+      <c r="D87" t="n">
+        <v>21.52</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>399.4400024414062</v>
+      </c>
+      <c r="C88" t="n">
+        <v>59.3189697265625</v>
+      </c>
+      <c r="D88" t="n">
+        <v>21.76</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>VCSH</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>75.33999633789062</v>
+      </c>
+      <c r="C89" t="n">
+        <v>3.631111145019531</v>
+      </c>
+      <c r="D89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>BSV</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>75.45999908447266</v>
+      </c>
+      <c r="C90" t="n">
+        <v>2.844619750976562</v>
+      </c>
+      <c r="D90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>VGSH</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>57.70999908447266</v>
+      </c>
+      <c r="C91" t="n">
+        <v>2.005947113037109</v>
+      </c>
+      <c r="D91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>VTEB</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>48.31000137329102</v>
+      </c>
+      <c r="C92" t="n">
+        <v>1.935108184814453</v>
+      </c>
+      <c r="D92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>BND</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>69.80000305175781</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1.994491577148438</v>
+      </c>
+      <c r="D93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>BNDX</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>48.27000045776367</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1.588729858398438</v>
+      </c>
+      <c r="D94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>VXUS</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>54.0099983215332</v>
+      </c>
+      <c r="C95" t="n">
+        <v>6.601516723632812</v>
+      </c>
+      <c r="D95" t="n">
+        <v>11.81</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>VTI</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>215.4100036621094</v>
+      </c>
+      <c r="C96" t="n">
+        <v>29.52322387695312</v>
+      </c>
+      <c r="D96" t="n">
+        <v>20.26</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>VTV</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>138.5899963378906</v>
+      </c>
+      <c r="C97" t="n">
+        <v>4.530548095703125</v>
+      </c>
+      <c r="D97" t="n">
+        <v>15.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try except for PE + cleaning up code
</commit_message>
<xml_diff>
--- a/stockdata.xlsx
+++ b/stockdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>PE Ratio</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Percent Change</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -468,6 +473,9 @@
         <v>-5.119999885559082</v>
       </c>
       <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>-46.54545350508256</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -482,6 +490,9 @@
         <v>5.511295318603516</v>
       </c>
       <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>15.77870002784953</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -498,6 +509,9 @@
       <c r="D4" t="n">
         <v>6.79</v>
       </c>
+      <c r="E4" t="n">
+        <v>5.443272499101457</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -509,11 +523,14 @@
         <v>47.61000061035156</v>
       </c>
       <c r="C5" t="n">
-        <v>6.427463531494141</v>
+        <v>6.427467346191406</v>
       </c>
       <c r="D5" t="n">
         <v>21.13</v>
       </c>
+      <c r="E5" t="n">
+        <v>15.60726559719682</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -525,11 +542,14 @@
         <v>67.55999755859375</v>
       </c>
       <c r="C6" t="n">
-        <v>22.26338577270508</v>
+        <v>22.26338195800781</v>
       </c>
       <c r="D6" t="n">
         <v>25.51</v>
       </c>
+      <c r="E6" t="n">
+        <v>49.15021059039083</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -546,6 +566,9 @@
       <c r="D7" t="n">
         <v>25.02</v>
       </c>
+      <c r="E7" t="n">
+        <v>17.64416291490852</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -557,11 +580,14 @@
         <v>68.75</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.272453308105469</v>
+        <v>-1.272445678710938</v>
       </c>
       <c r="D8" t="n">
         <v>23.44</v>
       </c>
+      <c r="E8" t="n">
+        <v>-1.817196852205637</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -573,11 +599,14 @@
         <v>86.68000030517578</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.441215515136719</v>
+        <v>-1.44122314453125</v>
       </c>
       <c r="D9" t="n">
         <v>8.02</v>
       </c>
+      <c r="E9" t="n">
+        <v>-1.63550060713103</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -594,6 +623,9 @@
       <c r="D10" t="n">
         <v>15.33</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.643133614697673</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -610,6 +642,9 @@
       <c r="D11" t="n">
         <v>22.6</v>
       </c>
+      <c r="E11" t="n">
+        <v>7.81474336437696</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -626,6 +661,9 @@
       <c r="D12" t="n">
         <v>13.19</v>
       </c>
+      <c r="E12" t="n">
+        <v>-8.682209757584568</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -642,6 +680,9 @@
       <c r="D13" t="n">
         <v>16.3</v>
       </c>
+      <c r="E13" t="n">
+        <v>17.02716501558704</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -658,6 +699,9 @@
       <c r="D14" t="n">
         <v>21.59</v>
       </c>
+      <c r="E14" t="n">
+        <v>-1.00794763509308</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -674,6 +718,9 @@
       <c r="D15" t="n">
         <v>21.82</v>
       </c>
+      <c r="E15" t="n">
+        <v>8.691383143203138</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -690,6 +737,9 @@
       <c r="D16" t="n">
         <v>29.98</v>
       </c>
+      <c r="E16" t="n">
+        <v>39.86794110166634</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -701,11 +751,14 @@
         <v>141.5899963378906</v>
       </c>
       <c r="C17" t="n">
-        <v>6.10919189453125</v>
+        <v>6.109207153320312</v>
       </c>
       <c r="D17" t="n">
         <v>18.02</v>
       </c>
+      <c r="E17" t="n">
+        <v>4.509279278700925</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -722,6 +775,9 @@
       <c r="D18" t="n">
         <v>10.2</v>
       </c>
+      <c r="E18" t="n">
+        <v>-38.22553843850461</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -738,6 +794,9 @@
       <c r="D19" t="n">
         <v>28.74</v>
       </c>
+      <c r="E19" t="n">
+        <v>9.860031557151387</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -754,6 +813,9 @@
       <c r="D20" t="n">
         <v>1.58</v>
       </c>
+      <c r="E20" t="n">
+        <v>-37.6157229903889</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -765,11 +827,14 @@
         <v>81.20999908447266</v>
       </c>
       <c r="C21" t="n">
-        <v>2.771461486816406</v>
+        <v>2.771438598632812</v>
       </c>
       <c r="D21" t="n">
         <v>3691.36</v>
       </c>
+      <c r="E21" t="n">
+        <v>3.533260403386836</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -781,9 +846,12 @@
         <v>49.95999908447266</v>
       </c>
       <c r="C22" t="n">
-        <v>2.388416290283203</v>
+        <v>2.388420104980469</v>
       </c>
       <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>5.020687049320145</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -795,9 +863,12 @@
         <v>87.62999725341797</v>
       </c>
       <c r="C23" t="n">
-        <v>-3.570449829101562</v>
+        <v>-3.570442199707031</v>
       </c>
       <c r="D23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>-3.914939687919113</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -812,6 +883,9 @@
         <v>0.7673416137695312</v>
       </c>
       <c r="D24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>0.8445071392286023</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -828,6 +902,9 @@
       <c r="D25" t="n">
         <v>15.63</v>
       </c>
+      <c r="E25" t="n">
+        <v>-6.42090010502763</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -844,6 +921,9 @@
       <c r="D26" t="n">
         <v>16.98</v>
       </c>
+      <c r="E26" t="n">
+        <v>5.392216294614858</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -860,6 +940,9 @@
       <c r="D27" t="n">
         <v>13.02</v>
       </c>
+      <c r="E27" t="n">
+        <v>16.76760065296373</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -876,6 +959,9 @@
       <c r="D28" t="n">
         <v>10.94</v>
       </c>
+      <c r="E28" t="n">
+        <v>10.22374098476149</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -887,11 +973,14 @@
         <v>436.5899963378906</v>
       </c>
       <c r="C29" t="n">
-        <v>64.81231689453125</v>
+        <v>64.81234741210938</v>
       </c>
       <c r="D29" t="n">
         <v>21.9</v>
       </c>
+      <c r="E29" t="n">
+        <v>17.43309410863696</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -903,11 +992,14 @@
         <v>247.3000030517578</v>
       </c>
       <c r="C30" t="n">
-        <v>11.22453308105469</v>
+        <v>11.22454833984375</v>
       </c>
       <c r="D30" t="n">
         <v>13.62</v>
       </c>
+      <c r="E30" t="n">
+        <v>4.754644379925567</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -924,6 +1016,9 @@
       <c r="D31" t="n">
         <v>11.65</v>
       </c>
+      <c r="E31" t="n">
+        <v>-0.1908718837237288</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -935,9 +1030,12 @@
         <v>43.75</v>
       </c>
       <c r="C32" t="n">
-        <v>1.571475982666016</v>
+        <v>1.571487426757812</v>
       </c>
       <c r="D32" t="inlineStr"/>
+      <c r="E32" t="n">
+        <v>3.725800960925197</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -954,6 +1052,9 @@
       <c r="D33" t="n">
         <v>120.13</v>
       </c>
+      <c r="E33" t="n">
+        <v>2.955986435294923</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -970,6 +1071,9 @@
       <c r="D34" t="n">
         <v>21.93</v>
       </c>
+      <c r="E34" t="n">
+        <v>16.17226250099335</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -986,6 +1090,9 @@
       <c r="D35" t="n">
         <v>14.72</v>
       </c>
+      <c r="E35" t="n">
+        <v>-28.04886802474985</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -997,11 +1104,14 @@
         <v>74.41000366210938</v>
       </c>
       <c r="C36" t="n">
-        <v>5.715110778808594</v>
+        <v>5.715103149414062</v>
       </c>
       <c r="D36" t="n">
         <v>9.279999999999999</v>
       </c>
+      <c r="E36" t="n">
+        <v>8.319544983339586</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1013,11 +1123,14 @@
         <v>101.9100036621094</v>
       </c>
       <c r="C37" t="n">
-        <v>4.792160034179688</v>
+        <v>4.792152404785156</v>
       </c>
       <c r="D37" t="n">
         <v>30.82</v>
       </c>
+      <c r="E37" t="n">
+        <v>4.934368236883486</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1034,6 +1147,9 @@
       <c r="D38" t="n">
         <v>11.31</v>
       </c>
+      <c r="E38" t="n">
+        <v>10.25669417872114</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1045,9 +1161,12 @@
         <v>83.51999664306641</v>
       </c>
       <c r="C39" t="n">
-        <v>6.973091125488281</v>
+        <v>6.973106384277344</v>
       </c>
       <c r="D39" t="inlineStr"/>
+      <c r="E39" t="n">
+        <v>9.109588071707062</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1059,9 +1178,12 @@
         <v>88.91000366210938</v>
       </c>
       <c r="C40" t="n">
-        <v>1.832321166992188</v>
+        <v>1.83233642578125</v>
       </c>
       <c r="D40" t="inlineStr"/>
+      <c r="E40" t="n">
+        <v>2.104255297524569</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1073,11 +1195,14 @@
         <v>21.80999946594238</v>
       </c>
       <c r="C41" t="n">
-        <v>1.259576797485352</v>
+        <v>1.259574890136719</v>
       </c>
       <c r="D41" t="n">
         <v>12.94</v>
       </c>
+      <c r="E41" t="n">
+        <v>6.129191567261516</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1094,6 +1219,9 @@
       <c r="D42" t="n">
         <v>5.81</v>
       </c>
+      <c r="E42" t="n">
+        <v>3.712450731307662</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1110,6 +1238,9 @@
       <c r="D43" t="n">
         <v>10.1</v>
       </c>
+      <c r="E43" t="n">
+        <v>8.896923007029486</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1126,6 +1257,9 @@
       <c r="D44" t="n">
         <v>13.33</v>
       </c>
+      <c r="E44" t="n">
+        <v>17.23678696014825</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1142,6 +1276,9 @@
       <c r="D45" t="n">
         <v>24.42</v>
       </c>
+      <c r="E45" t="n">
+        <v>2.725820641488185</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1153,11 +1290,14 @@
         <v>82.5</v>
       </c>
       <c r="C46" t="n">
-        <v>13.54653930664062</v>
+        <v>13.54653167724609</v>
       </c>
       <c r="D46" t="n">
         <v>24.52</v>
       </c>
+      <c r="E46" t="n">
+        <v>19.64590325440654</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1174,6 +1314,9 @@
       <c r="D47" t="n">
         <v>12.3</v>
       </c>
+      <c r="E47" t="n">
+        <v>15.86315325557167</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1190,6 +1333,9 @@
       <c r="D48" t="n">
         <v>12.87</v>
       </c>
+      <c r="E48" t="n">
+        <v>25.41581725775765</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1206,6 +1352,9 @@
       <c r="D49" t="n">
         <v>23.19</v>
       </c>
+      <c r="E49" t="n">
+        <v>7.60403265061219</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1222,6 +1371,9 @@
       <c r="D50" t="n">
         <v>15</v>
       </c>
+      <c r="E50" t="n">
+        <v>0.4402791448247157</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1233,11 +1385,14 @@
         <v>134.9900054931641</v>
       </c>
       <c r="C51" t="n">
-        <v>26.37348937988281</v>
+        <v>26.37348175048828</v>
       </c>
       <c r="D51" t="n">
         <v>19.91</v>
       </c>
+      <c r="E51" t="n">
+        <v>24.28127953438272</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1249,9 +1404,12 @@
         <v>102.7600021362305</v>
       </c>
       <c r="C52" t="n">
-        <v>3.523262023925781</v>
+        <v>3.523269653320312</v>
       </c>
       <c r="D52" t="inlineStr"/>
+      <c r="E52" t="n">
+        <v>3.55036846253182</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1263,11 +1421,14 @@
         <v>273.6400146484375</v>
       </c>
       <c r="C53" t="n">
-        <v>63.31600952148438</v>
+        <v>63.31599426269531</v>
       </c>
       <c r="D53" t="n">
         <v>30.21</v>
       </c>
+      <c r="E53" t="n">
+        <v>30.10402432711746</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1279,11 +1440,14 @@
         <v>151.8300018310547</v>
       </c>
       <c r="C54" t="n">
-        <v>6.307769775390625</v>
+        <v>6.3077392578125</v>
       </c>
       <c r="D54" t="n">
         <v>15.79</v>
       </c>
+      <c r="E54" t="n">
+        <v>4.33455276620495</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1300,6 +1464,9 @@
       <c r="D55" t="n">
         <v>11.13</v>
       </c>
+      <c r="E55" t="n">
+        <v>-0.7962927924961961</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1311,9 +1478,12 @@
         <v>110.1500015258789</v>
       </c>
       <c r="C56" t="n">
-        <v>5.037483215332031</v>
+        <v>5.037498474121094</v>
       </c>
       <c r="D56" t="inlineStr"/>
+      <c r="E56" t="n">
+        <v>4.792482652268883</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1325,11 +1495,14 @@
         <v>104.2399978637695</v>
       </c>
       <c r="C57" t="n">
-        <v>1.964340209960938</v>
+        <v>1.964347839355469</v>
       </c>
       <c r="D57" t="n">
         <v>11.71</v>
       </c>
+      <c r="E57" t="n">
+        <v>1.920640777043766</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1346,6 +1519,9 @@
       <c r="D58" t="n">
         <v>13.6</v>
       </c>
+      <c r="E58" t="n">
+        <v>17.25059076969788</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1357,11 +1533,14 @@
         <v>113.4199981689453</v>
       </c>
       <c r="C59" t="n">
-        <v>7.199058532714844</v>
+        <v>7.199066162109375</v>
       </c>
       <c r="D59" t="n">
         <v>26.11</v>
       </c>
+      <c r="E59" t="n">
+        <v>6.777445863161955</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1376,6 +1555,9 @@
         <v>0.4086074829101562</v>
       </c>
       <c r="D60" t="inlineStr"/>
+      <c r="E60" t="n">
+        <v>1.885469445613296</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1392,6 +1574,9 @@
       <c r="D61" t="n">
         <v>32.91</v>
       </c>
+      <c r="E61" t="n">
+        <v>52.22966376014038</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1403,11 +1588,14 @@
         <v>58.81999969482422</v>
       </c>
       <c r="C62" t="n">
-        <v>2.429946899414062</v>
+        <v>2.429950714111328</v>
       </c>
       <c r="D62" t="n">
         <v>13.23</v>
       </c>
+      <c r="E62" t="n">
+        <v>4.309183549286232</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1419,11 +1607,14 @@
         <v>53.59000015258789</v>
       </c>
       <c r="C63" t="n">
-        <v>3.172592163085938</v>
+        <v>3.172588348388672</v>
       </c>
       <c r="D63" t="n">
         <v>23.37</v>
       </c>
+      <c r="E63" t="n">
+        <v>6.292644217259145</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1438,6 +1629,9 @@
         <v>1.685844421386719</v>
       </c>
       <c r="D64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>3.485010442792541</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1454,6 +1648,9 @@
       <c r="D65" t="n">
         <v>7.92</v>
       </c>
+      <c r="E65" t="n">
+        <v>8.119083372938375</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1468,6 +1665,9 @@
         <v>2.395439147949219</v>
       </c>
       <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>2.797934211586295</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1482,6 +1682,9 @@
         <v>5.75</v>
       </c>
       <c r="D67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>22.06446706767831</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1493,11 +1696,14 @@
         <v>70.25</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.6469039916992188</v>
+        <v>-0.6468963623046875</v>
       </c>
       <c r="D68" t="n">
         <v>13.33</v>
       </c>
+      <c r="E68" t="n">
+        <v>-0.9124466591581816</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1509,442 +1715,510 @@
         <v>91.48000335693359</v>
       </c>
       <c r="C69" t="n">
-        <v>4.101837158203125</v>
+        <v>4.101860046386719</v>
       </c>
       <c r="D69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>4.694377668118302</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>SPY</t>
+          <t>XLK</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>434.6900024414062</v>
+        <v>171.7599945068359</v>
       </c>
       <c r="C70" t="n">
-        <v>64.17276000976562</v>
+        <v>51.88981628417969</v>
       </c>
       <c r="D70" t="n">
-        <v>21.9</v>
+        <v>32.54</v>
+      </c>
+      <c r="E70" t="n">
+        <v>43.28834498585251</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>XLK</t>
+          <t>XLU</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>171.7599945068359</v>
+        <v>61.86000061035156</v>
       </c>
       <c r="C71" t="n">
-        <v>51.88980102539062</v>
+        <v>-3.144767761230469</v>
       </c>
       <c r="D71" t="n">
-        <v>32.54</v>
+        <v>21.76</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-4.837749352869411</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>XLU</t>
+          <t>MOAT</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>61.86000061035156</v>
+        <v>75.30999755859375</v>
       </c>
       <c r="C72" t="n">
-        <v>-3.144767761230469</v>
+        <v>14.03970336914062</v>
       </c>
       <c r="D72" t="n">
-        <v>21.76</v>
+        <v>23.97</v>
+      </c>
+      <c r="E72" t="n">
+        <v>22.91437238040449</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MOAT</t>
+          <t>SMH</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>75.30999755859375</v>
+        <v>149.5099945068359</v>
       </c>
       <c r="C73" t="n">
-        <v>14.03970336914062</v>
+        <v>54.88582611083984</v>
       </c>
       <c r="D73" t="n">
-        <v>23.97</v>
+        <v>12.93</v>
+      </c>
+      <c r="E73" t="n">
+        <v>58.00402480806612</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>SMH</t>
+          <t>VIG</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>149.5099945068359</v>
+        <v>157.7400054931641</v>
       </c>
       <c r="C74" t="n">
-        <v>54.88582611083984</v>
+        <v>14.30448913574219</v>
       </c>
       <c r="D74" t="n">
-        <v>12.93</v>
+        <v>22.21</v>
+      </c>
+      <c r="E74" t="n">
+        <v>9.972766507911009</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>VIG</t>
+          <t>ESGV</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>157.7400054931641</v>
+        <v>76.45999908447266</v>
       </c>
       <c r="C75" t="n">
-        <v>14.30448913574219</v>
+        <v>12.44647979736328</v>
       </c>
       <c r="D75" t="n">
-        <v>22.21</v>
+        <v>22.5</v>
+      </c>
+      <c r="E75" t="n">
+        <v>19.44351745689707</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ESGV</t>
+          <t>VEU</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>76.45999908447266</v>
+        <v>52.43999862670898</v>
       </c>
       <c r="C76" t="n">
-        <v>12.44647979736328</v>
+        <v>6.538074493408203</v>
       </c>
       <c r="D76" t="n">
-        <v>22.5</v>
+        <v>11.97</v>
+      </c>
+      <c r="E76" t="n">
+        <v>14.24357391734039</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>VEU</t>
+          <t>VEA</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>52.43999862670898</v>
+        <v>44.18999862670898</v>
       </c>
       <c r="C77" t="n">
-        <v>6.538074493408203</v>
+        <v>5.960308074951172</v>
       </c>
       <c r="D77" t="n">
-        <v>11.97</v>
+        <v>12.17</v>
+      </c>
+      <c r="E77" t="n">
+        <v>15.59078294625933</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>VEA</t>
+          <t>VWO</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>44.18999862670898</v>
+        <v>39.5099983215332</v>
       </c>
       <c r="C78" t="n">
-        <v>5.960304260253906</v>
+        <v>3.106525421142578</v>
       </c>
       <c r="D78" t="n">
-        <v>12.17</v>
+        <v>10.76</v>
+      </c>
+      <c r="E78" t="n">
+        <v>8.533596312755215</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>VWO</t>
+          <t>VGK</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>39.5099983215332</v>
+        <v>58.2400016784668</v>
       </c>
       <c r="C79" t="n">
-        <v>3.106521606445312</v>
+        <v>8.653205871582031</v>
       </c>
       <c r="D79" t="n">
-        <v>10.76</v>
+        <v>12.53</v>
+      </c>
+      <c r="E79" t="n">
+        <v>17.45062517304374</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>VGK</t>
+          <t>VUG</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>58.2400016784668</v>
+        <v>279.8900146484375</v>
       </c>
       <c r="C80" t="n">
-        <v>8.653209686279297</v>
+        <v>70.10682678222656</v>
       </c>
       <c r="D80" t="n">
-        <v>12.53</v>
+        <v>33.69</v>
+      </c>
+      <c r="E80" t="n">
+        <v>33.41870599608637</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>VUG</t>
+          <t>VHT</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>279.8900146484375</v>
+        <v>231.4600067138672</v>
       </c>
       <c r="C81" t="n">
-        <v>70.1068115234375</v>
+        <v>-4.196975708007812</v>
       </c>
       <c r="D81" t="n">
-        <v>33.69</v>
+        <v>20.99</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-1.780968110885148</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>VHT</t>
+          <t>VYM</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>231.4600067138672</v>
+        <v>103.8199996948242</v>
       </c>
       <c r="C82" t="n">
-        <v>-4.19696044921875</v>
+        <v>0.5161590576171875</v>
       </c>
       <c r="D82" t="n">
-        <v>20.99</v>
+        <v>14.22</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.4996513725272689</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>VYM</t>
+          <t>VGT</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>103.8199996948242</v>
+        <v>427.8800048828125</v>
       </c>
       <c r="C83" t="n">
-        <v>0.5161666870117188</v>
+        <v>119.9216918945312</v>
       </c>
       <c r="D83" t="n">
-        <v>14.22</v>
+        <v>31.74</v>
+      </c>
+      <c r="E83" t="n">
+        <v>38.94088480056541</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>VGT</t>
+          <t>VCIT</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>427.8800048828125</v>
+        <v>76.05000305175781</v>
       </c>
       <c r="C84" t="n">
-        <v>119.9217529296875</v>
-      </c>
-      <c r="D84" t="n">
-        <v>31.74</v>
+        <v>3.864524841308594</v>
+      </c>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="n">
+        <v>5.353604266556184</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>VCIT</t>
+          <t>VO</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>76.05000305175781</v>
+        <v>207.8000030517578</v>
       </c>
       <c r="C85" t="n">
-        <v>3.864532470703125</v>
-      </c>
-      <c r="D85" t="inlineStr"/>
+        <v>10.20899963378906</v>
+      </c>
+      <c r="D85" t="n">
+        <v>16.87</v>
+      </c>
+      <c r="E85" t="n">
+        <v>5.166733027917133</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>VO</t>
+          <t>VNQ</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>207.8000030517578</v>
+        <v>77.58999633789062</v>
       </c>
       <c r="C86" t="n">
-        <v>10.20899963378906</v>
+        <v>-0.483062744140625</v>
       </c>
       <c r="D86" t="n">
-        <v>16.87</v>
+        <v>21.52</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-0.6187316723853125</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>VNQ</t>
+          <t>VOO</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>77.58999633789062</v>
+        <v>399.4400024414062</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.4830703735351562</v>
+        <v>59.3189697265625</v>
       </c>
       <c r="D87" t="n">
-        <v>21.52</v>
+        <v>21.76</v>
+      </c>
+      <c r="E87" t="n">
+        <v>17.44054734077422</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>VOO</t>
+          <t>VCSH</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>399.4400024414062</v>
+        <v>75.33999633789062</v>
       </c>
       <c r="C88" t="n">
-        <v>59.3189697265625</v>
-      </c>
-      <c r="D88" t="n">
-        <v>21.76</v>
+        <v>3.631111145019531</v>
+      </c>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>5.063683719602039</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>VCSH</t>
+          <t>BSV</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>75.33999633789062</v>
+        <v>75.45999908447266</v>
       </c>
       <c r="C89" t="n">
-        <v>3.631111145019531</v>
+        <v>2.844612121582031</v>
       </c>
       <c r="D89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>3.917368261131408</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>BSV</t>
+          <t>VGSH</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>75.45999908447266</v>
+        <v>57.70999908447266</v>
       </c>
       <c r="C90" t="n">
-        <v>2.844619750976562</v>
+        <v>2.005943298339844</v>
       </c>
       <c r="D90" t="inlineStr"/>
+      <c r="E90" t="n">
+        <v>3.601072255925772</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>VGSH</t>
+          <t>VTEB</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>57.70999908447266</v>
+        <v>48.31000137329102</v>
       </c>
       <c r="C91" t="n">
-        <v>2.005947113037109</v>
+        <v>1.935111999511719</v>
       </c>
       <c r="D91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>4.172758200919494</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>VTEB</t>
+          <t>BND</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>48.31000137329102</v>
+        <v>69.80000305175781</v>
       </c>
       <c r="C92" t="n">
-        <v>1.935108184814453</v>
+        <v>1.994491577148438</v>
       </c>
       <c r="D92" t="inlineStr"/>
+      <c r="E92" t="n">
+        <v>2.941488875716689</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>BND</t>
+          <t>BNDX</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>69.80000305175781</v>
+        <v>48.27000045776367</v>
       </c>
       <c r="C93" t="n">
-        <v>1.994491577148438</v>
+        <v>1.588722229003906</v>
       </c>
       <c r="D93" t="inlineStr"/>
+      <c r="E93" t="n">
+        <v>3.40333917425833</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>BNDX</t>
+          <t>VXUS</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>48.27000045776367</v>
+        <v>54.0099983215332</v>
       </c>
       <c r="C94" t="n">
-        <v>1.588729858398438</v>
-      </c>
-      <c r="D94" t="inlineStr"/>
+        <v>6.601516723632812</v>
+      </c>
+      <c r="D94" t="n">
+        <v>11.81</v>
+      </c>
+      <c r="E94" t="n">
+        <v>13.92475882190072</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>VXUS</t>
+          <t>VTI</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>54.0099983215332</v>
+        <v>215.4100036621094</v>
       </c>
       <c r="C95" t="n">
-        <v>6.601516723632812</v>
+        <v>29.52323913574219</v>
       </c>
       <c r="D95" t="n">
-        <v>11.81</v>
+        <v>20.26</v>
+      </c>
+      <c r="E95" t="n">
+        <v>15.88237829141109</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>VTI</t>
+          <t>VTV</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>215.4100036621094</v>
+        <v>138.5899963378906</v>
       </c>
       <c r="C96" t="n">
-        <v>29.52322387695312</v>
+        <v>4.530532836914062</v>
       </c>
       <c r="D96" t="n">
-        <v>20.26</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>VTV</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
-        <v>138.5899963378906</v>
-      </c>
-      <c r="C97" t="n">
-        <v>4.530548095703125</v>
-      </c>
-      <c r="D97" t="n">
         <v>15.49</v>
+      </c>
+      <c r="E96" t="n">
+        <v>3.37949497827213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>